<commit_message>
Implementação no product backlog
</commit_message>
<xml_diff>
--- a/Product Backlog/Product Backlog - MorumByte.xlsx
+++ b/Product Backlog/Product Backlog - MorumByte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanr\Documents\GIT\MorumByte\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D5745C-4F6C-4C89-9374-D7E3D6105E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FD8E87-5541-41A7-B7CD-C9204BF1C4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D8726E2A-0C03-44E9-843D-7D8F8FD916AD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="87">
   <si>
     <t>Nº</t>
   </si>
@@ -310,13 +310,32 @@
   <si>
     <t>Função para alertar quando o usuário digitar dados que não correspondem a
 dados salvos no banco de dados</t>
+  </si>
+  <si>
+    <t>Prototipagem do site</t>
+  </si>
+  <si>
+    <t>Design completo do site, desde a parte institucional até a parte funcional 
+(Quis, Dashboard).</t>
+  </si>
+  <si>
+    <t>Essencial</t>
+  </si>
+  <si>
+    <t>Importante</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Essencial</t>
+  </si>
+  <si>
+    <t>Desejável</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,6 +372,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -425,52 +451,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -480,51 +524,7 @@
   <dxfs count="11">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -570,6 +570,23 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -582,6 +599,36 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -673,16 +720,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AD658527-F84D-4B86-8092-55E82BAA1BF4}" name="Tabela2" displayName="Tabela2" ref="C10:J45" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8" headerRowCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AD658527-F84D-4B86-8092-55E82BAA1BF4}" name="Tabela2" displayName="Tabela2" ref="C10:J46" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8" headerRowCellStyle="Normal">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{0511EB12-3CC2-4C21-9082-E34484A2C207}" name="Nº" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{DC812239-49D3-4532-BADA-C29B2E9D97E7}" name="Requisitos" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{DA9D9EDB-AE02-4820-A9BB-E4D99EC43748}" name=" Descrição" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{0BB06448-83F6-4B81-AB3C-9F6118E25B7E}" name=" Classificação" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{C2258953-CA3A-4D3F-9A2F-63BF385276F0}" name="Tamanho" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{7EE4BA1F-0742-4027-8F50-977929B6A942}" name=" Tam (#)" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{F3B08DFA-B4B2-475C-9968-F458300DAF18}" name=" Prioridade" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{5290F820-6BEE-473A-B375-64C13757AE85}" name="Sprint" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0511EB12-3CC2-4C21-9082-E34484A2C207}" name="Nº" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{DC812239-49D3-4532-BADA-C29B2E9D97E7}" name="Requisitos" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{DA9D9EDB-AE02-4820-A9BB-E4D99EC43748}" name=" Descrição" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{0BB06448-83F6-4B81-AB3C-9F6118E25B7E}" name=" Classificação" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{C2258953-CA3A-4D3F-9A2F-63BF385276F0}" name="Tamanho" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{7EE4BA1F-0742-4027-8F50-977929B6A942}" name=" Tam (#)" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{F3B08DFA-B4B2-475C-9968-F458300DAF18}" name=" Prioridade" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{5290F820-6BEE-473A-B375-64C13757AE85}" name="Sprint" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -985,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40DC9970-5FA2-4D2C-A477-0542CEE05661}">
-  <dimension ref="C4:M45"/>
+  <dimension ref="C4:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1006,44 +1053,44 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="6"/>
+      <c r="M4" s="5"/>
     </row>
     <row r="5" spans="3:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
     </row>
     <row r="6" spans="3:13" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
     </row>
     <row r="7" spans="3:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
     </row>
     <row r="8" spans="3:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
     </row>
     <row r="9" spans="3:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
@@ -1054,471 +1101,577 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="L9" s="8" t="s">
+      <c r="L9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="9"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="3:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="3:13" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="10"/>
-      <c r="D11" s="11" t="s">
+      <c r="C11" s="20"/>
+      <c r="D11" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
+      <c r="F11" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
     </row>
     <row r="12" spans="3:13" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="10"/>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="20"/>
+      <c r="D12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
+      <c r="F12" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
     </row>
     <row r="13" spans="3:13" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="10"/>
-      <c r="D13" s="12" t="s">
+      <c r="C13" s="20"/>
+      <c r="D13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="F13" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
     </row>
     <row r="14" spans="3:13" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="13"/>
-      <c r="D14" s="14" t="s">
+      <c r="C14" s="21"/>
+      <c r="D14" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
+      <c r="F14" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
     </row>
     <row r="15" spans="3:13" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="10"/>
-      <c r="D15" s="12" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+      <c r="F15" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
     </row>
     <row r="16" spans="3:13" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="10"/>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="20"/>
+      <c r="D16" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
+      <c r="F16" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
     </row>
     <row r="17" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="10"/>
-      <c r="D17" s="12" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
+      <c r="F17" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
     </row>
     <row r="18" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="10"/>
-      <c r="D18" s="12" t="s">
+      <c r="C18" s="20"/>
+      <c r="D18" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
+      <c r="F18" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
     </row>
     <row r="19" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="10"/>
-      <c r="D19" s="12" t="s">
+      <c r="C19" s="20"/>
+      <c r="D19" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
+      <c r="F19" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
     </row>
     <row r="20" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="10"/>
-      <c r="D20" s="12" t="s">
+      <c r="C20" s="20"/>
+      <c r="D20" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
+      <c r="F20" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
     </row>
     <row r="21" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="10"/>
-      <c r="D21" s="12" t="s">
+      <c r="C21" s="20"/>
+      <c r="D21" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
+      <c r="F21" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
     </row>
     <row r="22" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="10"/>
-      <c r="D22" s="12" t="s">
+      <c r="C22" s="20"/>
+      <c r="D22" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
+      <c r="F22" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
     </row>
     <row r="23" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="10"/>
-      <c r="D23" s="12" t="s">
+      <c r="C23" s="20"/>
+      <c r="D23" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-    </row>
-    <row r="24" spans="3:10" s="13" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="15" t="s">
+      <c r="F23" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+    </row>
+    <row r="24" spans="3:10" s="12" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="21"/>
+      <c r="D24" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="13" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="25" spans="3:10" s="13" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="15" t="s">
+      <c r="F24" s="21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" s="12" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="21"/>
+      <c r="D25" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="13" t="s">
         <v>42</v>
       </c>
+      <c r="F25" s="21" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="26" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="10"/>
-      <c r="D26" s="12" t="s">
+      <c r="C26" s="20"/>
+      <c r="D26" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-    </row>
-    <row r="27" spans="3:10" s="13" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="15" t="s">
+      <c r="F26" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+    </row>
+    <row r="27" spans="3:10" s="12" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="21"/>
+      <c r="D27" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="13" t="s">
         <v>44</v>
       </c>
+      <c r="F27" s="21" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="28" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="10"/>
-      <c r="D28" s="11" t="s">
+      <c r="C28" s="20"/>
+      <c r="D28" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
+      <c r="F28" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
     </row>
     <row r="29" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="10"/>
-      <c r="D29" s="11" t="s">
+      <c r="C29" s="20"/>
+      <c r="D29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
+      <c r="F29" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
     </row>
     <row r="30" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="10"/>
-      <c r="D30" s="11" t="s">
+      <c r="C30" s="20"/>
+      <c r="D30" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
+      <c r="F30" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
     </row>
     <row r="31" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="10"/>
-      <c r="D31" s="11" t="s">
+      <c r="C31" s="20"/>
+      <c r="D31" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
+      <c r="F31" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
     </row>
     <row r="32" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="10"/>
-      <c r="D32" s="11" t="s">
+      <c r="C32" s="20"/>
+      <c r="D32" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
+      <c r="F32" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
     </row>
     <row r="33" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="10"/>
-      <c r="D33" s="12" t="s">
+      <c r="C33" s="20"/>
+      <c r="D33" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
+      <c r="F33" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
     </row>
     <row r="34" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="10"/>
-      <c r="D34" s="12" t="s">
+      <c r="C34" s="20"/>
+      <c r="D34" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-    </row>
-    <row r="35" spans="3:10" s="16" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D35" s="15" t="s">
+      <c r="F34" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+    </row>
+    <row r="35" spans="3:10" s="14" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="22"/>
+      <c r="D35" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="13" t="s">
         <v>66</v>
       </c>
+      <c r="F35" s="21" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="36" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="10"/>
-      <c r="D36" s="12" t="s">
+      <c r="C36" s="20"/>
+      <c r="D36" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
+      <c r="F36" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
     </row>
     <row r="37" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="10"/>
-      <c r="D37" s="11" t="s">
+      <c r="C37" s="20"/>
+      <c r="D37" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-    </row>
-    <row r="38" spans="3:10" s="13" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="15" t="s">
+      <c r="F37" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+    </row>
+    <row r="38" spans="3:10" s="12" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="21"/>
+      <c r="D38" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="13" t="s">
         <v>68</v>
       </c>
+      <c r="F38" s="21" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="39" spans="3:10" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="10"/>
-      <c r="D39" s="12" t="s">
+      <c r="C39" s="20"/>
+      <c r="D39" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E39" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
+      <c r="F39" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
     </row>
     <row r="40" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="10"/>
-      <c r="D40" s="12" t="s">
+      <c r="C40" s="20"/>
+      <c r="D40" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="E40" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-    </row>
-    <row r="41" spans="3:10" s="13" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="14" t="s">
+      <c r="F40" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+    </row>
+    <row r="41" spans="3:10" s="12" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="21"/>
+      <c r="D41" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="E41" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="J41" s="10"/>
-    </row>
-    <row r="42" spans="3:10" s="13" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D42" s="14" t="s">
+      <c r="F41" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="J41" s="9"/>
+    </row>
+    <row r="42" spans="3:10" s="12" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="21"/>
+      <c r="D42" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E42" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="J42" s="10"/>
-    </row>
-    <row r="43" spans="3:10" s="13" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="14" t="s">
+      <c r="F42" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J42" s="9"/>
+    </row>
+    <row r="43" spans="3:10" s="12" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="21"/>
+      <c r="D43" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="J43" s="10"/>
-    </row>
-    <row r="44" spans="3:10" s="13" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="14" t="s">
+      <c r="F43" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J43" s="9"/>
+    </row>
+    <row r="44" spans="3:10" s="12" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="21"/>
+      <c r="D44" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E44" s="15" t="s">
+      <c r="E44" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="J44" s="10"/>
-    </row>
-    <row r="45" spans="3:10" s="13" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="14" t="s">
+      <c r="F44" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="J44" s="9"/>
+    </row>
+    <row r="45" spans="3:10" s="12" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="21"/>
+      <c r="D45" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="E45" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="J45" s="10"/>
+      <c r="F45" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="J45" s="9"/>
+    </row>
+    <row r="46" spans="3:10" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="21"/>
+      <c r="D46" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F46" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>